<commit_message>
Import Master data dan Add Sensor pemasangan dan maintennace
</commit_message>
<xml_diff>
--- a/public/MasterGps/template-gps (2).xlsx
+++ b/public/MasterGps/template-gps (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dowloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A3FB72-0458-4F7F-9A3F-3537AA50CD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3942E2B6-176A-48DF-A8C9-6B3440B87F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Merk</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Sewa</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Ruptela</t>
@@ -419,7 +416,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,13 +450,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2">
-        <v>1173828738287720</v>
+        <v>873652413245321</v>
       </c>
       <c r="D2" s="1">
         <v>44488</v>
@@ -468,19 +465,16 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>638282888717</v>
+        <v>152635423178765</v>
       </c>
       <c r="D3" s="1">
         <v>44489</v>

</xml_diff>